<commit_message>
Refactor person status handling: Remove deprecated route for person status API, update PersonStatusDropdown to use metadata service for fetching options, and integrate FSM license options into UserForm with improved loading and error handling.
</commit_message>
<xml_diff>
--- a/API_Mappings.xlsx
+++ b/API_Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learnings\fsm-webtools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D6D7FC-AC03-4237-BBE4-C6B38C3099F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208680E6-4B60-4F26-B8BB-930BCA19A655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="10440" windowWidth="19410" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GET" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Drop Down</t>
   </si>
@@ -114,9 +114,6 @@
     <t>USER_ROLE</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Return Columns</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>Places~Location</t>
   </si>
   <si>
-    <t>place_relationship</t>
-  </si>
-  <si>
     <t>code_value_description_message_id</t>
   </si>
   <si>
@@ -157,13 +151,149 @@
   </si>
   <si>
     <t>team_id, description</t>
+  </si>
+  <si>
+    <t>PLACE_RELATIONSHIP</t>
+  </si>
+  <si>
+    <t>Queries</t>
+  </si>
+  <si>
+    <t>select code_name,code_value,message_id from metrix_code_table mxt
+where mxt.code_name in ('METRIX_USER_TYPE', 'PERSON_STATUS') and mxt.active = 'Y'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select user_role, description from user_role </t>
+  </si>
+  <si>
+    <r>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  place_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>status </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> place </t>
+    </r>
+  </si>
+  <si>
+    <t>select top 16 l.place_id, l.location, l.description,l.usable from location l 
+join place p on l.place_id = p.place_id
+where l.usable &lt;&gt; 'U'</t>
+  </si>
+  <si>
+    <t>select code_name,code_value,description from GLOBAL_CODE_TABLE
+where code_name in ('PLACE_RELATIONSHIP','LOCALE_CODE','POSTING_GROUP','ACCESS_GROUP','PERSON_GROUP','ADDRESS_TYPE')
+and active = 'Y'</t>
+  </si>
+  <si>
+    <t>select currency, description from currency where active = 'Y'</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/metrix_code_table?$select=code_name,code_value,message_id&amp;$filter=code_name eq 'METRIX_USER_TYPE' or code_name eq 'PERSON_STATUS' and active eq 'Y'</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/GLOBAL_CODE_TABLE?$select=code_name,code_value,description&amp;$filter=(code_name eq 'PLACE_RELATIONSHIP' or code_name eq 'LOCALE_CODE' or code_name eq 'POSTING_GROUP' or code_name eq 'ACCESS_GROUP' or code_name eq 'PERSON_GROUP' or code_name eq 'ADDRESS_TYPE') and active eq 'Y'</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/currency?$select=currency,description&amp;$filter=active eq 'Y'</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/user_role?$select=user_role,description</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/place?$select=place_id,name,status&amp;$filter=whos_place ne 'CUST'</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/location?$select=place_id,location,description,usable&amp;$filter=usable ne 'U'</t>
+  </si>
+  <si>
+    <t>select team_id,description,status,access_group from team where status = 'ACTIVE'</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/team?$select=team_id,description,status,access_group&amp;$filter=status eq 'ACTIVE'</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/C_LELY_PLACE_ADDRESS_VIEW?$select=place_id,whos_place,name,address_id,address_type,address_name,address,second_address,third_address,fourth_address,city,state_prov,zippost,country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+select place_id,whos_place,name,address_id,address_type,address_name,address, second_address,third_address,fourth_address,city,state_prov,zippost, country from C_LELY_PLACE_ADDRESS_VIEW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,16 +301,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -188,17 +361,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -215,15 +452,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{424D25A8-52B5-4123-8FA7-B9CAEE9EA596}" name="Table1" displayName="Table1" ref="A1:F20" totalsRowShown="0">
-  <autoFilter ref="A1:F20" xr:uid="{424D25A8-52B5-4123-8FA7-B9CAEE9EA596}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{424D25A8-52B5-4123-8FA7-B9CAEE9EA596}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0">
+  <autoFilter ref="A1:E20" xr:uid="{424D25A8-52B5-4123-8FA7-B9CAEE9EA596}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{344A0604-DC1E-4AB1-B558-BD53CD110DB2}" name="Drop Down"/>
     <tableColumn id="2" xr3:uid="{2F9C1649-6215-4685-92CE-39BC1269EAE4}" name="Table "/>
     <tableColumn id="3" xr3:uid="{61167488-83F5-475C-8A41-D1C0FD794760}" name="Code Name"/>
     <tableColumn id="6" xr3:uid="{F28DC5B5-BD70-4304-9444-35066E35D9EB}" name="Clauses"/>
     <tableColumn id="5" xr3:uid="{C1EED0B2-E6F2-4369-A8FD-40FAE54F33CC}" name="Return Columns"/>
-    <tableColumn id="4" xr3:uid="{9DC78172-273C-4D92-B143-4B36339849BB}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -492,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,10 +741,11 @@
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,17 +759,20 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -541,12 +781,18 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
@@ -555,187 +801,323 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
+      <c r="F16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F10"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{03D74FDA-8085-403F-8977-93F9ED7C5E15}"/>
+    <hyperlink ref="G4" r:id="rId2" display="https://lely-fsm-dev.ifs.cloud/odata/GLOBAL_CODE_TABLE?$select=code_name,code_value,description&amp;$filter=(code_name eq 'PLACE_RELATIONSHIP' or code_name eq 'LOCALE_CODE' or code_name eq 'POSTING_GROUP' or code_name eq 'ACCESS_GROUP' or code_name eq 'PERSON_GROUP' or code_name eq 'ADDRESS_TYPE') and active eq 'Y'" xr:uid="{CEA0CF45-549C-48BA-B180-779DDEDEE112}"/>
+    <hyperlink ref="G11" r:id="rId3" xr:uid="{F087DE0D-88EB-4BE9-9A29-4A1E7D02C0B0}"/>
+    <hyperlink ref="G12" r:id="rId4" xr:uid="{DE6DED64-57E6-4ED9-986A-542A27FF5942}"/>
+    <hyperlink ref="G13" r:id="rId5" xr:uid="{62D799AB-4983-4190-AEDB-16209CD9D356}"/>
+    <hyperlink ref="G14" r:id="rId6" xr:uid="{DD4FCA2E-16A8-4B92-B9C6-2E67018B733C}"/>
+    <hyperlink ref="G16" r:id="rId7" xr:uid="{89F98415-E335-4312-A443-E9E32386A825}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{E41EF9C3-8B68-4A2E-B747-49B9CBD836FF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement user role management in UserForm: Introduce useUserRoleOptions hook for dynamic role selection, enhance loading/error handling, and refactor MultiSelect component for improved filtering. Update API mappings for user roles.
</commit_message>
<xml_diff>
--- a/API_Mappings.xlsx
+++ b/API_Mappings.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learnings\fsm-webtools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208680E6-4B60-4F26-B8BB-930BCA19A655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F73709-5F3C-4BC7-9A34-B9564018FF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GET" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -264,9 +265,6 @@
     <t>https://lely-fsm-dev.ifs.cloud/odata/GLOBAL_CODE_TABLE?$select=code_name,code_value,description&amp;$filter=(code_name eq 'PLACE_RELATIONSHIP' or code_name eq 'LOCALE_CODE' or code_name eq 'POSTING_GROUP' or code_name eq 'ACCESS_GROUP' or code_name eq 'PERSON_GROUP' or code_name eq 'ADDRESS_TYPE') and active eq 'Y'</t>
   </si>
   <si>
-    <t>https://lely-fsm-dev.ifs.cloud/odata/currency?$select=currency,description&amp;$filter=active eq 'Y'</t>
-  </si>
-  <si>
     <t>https://lely-fsm-dev.ifs.cloud/odata/user_role?$select=user_role,description</t>
   </si>
   <si>
@@ -287,6 +285,9 @@
   <si>
     <t xml:space="preserve">
 select place_id,whos_place,name,address_id,address_type,address_name,address, second_address,third_address,fourth_address,city,state_prov,zippost, country from C_LELY_PLACE_ADDRESS_VIEW</t>
+  </si>
+  <si>
+    <t>https://lely-fsm-dev.ifs.cloud/odata/currency?$select=currency,description,format_override&amp;$filter=active eq 'Y'</t>
   </si>
 </sst>
 </file>
@@ -333,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +350,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,7 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -398,7 +405,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -415,6 +421,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -430,9 +439,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -449,6 +457,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>27200</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>189167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B18D8AC8-C5A9-D787-E38E-77467E069673}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11000000" cy="10666667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -730,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +799,7 @@
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="79.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -761,15 +818,15 @@
       <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -789,7 +846,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -805,7 +862,7 @@
       <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -826,16 +883,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="6"/>
@@ -843,16 +900,16 @@
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="6"/>
@@ -860,16 +917,16 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="6"/>
@@ -877,16 +934,16 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="6"/>
@@ -894,45 +951,45 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -941,15 +998,15 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="19" t="s">
-        <v>53</v>
+      <c r="G11" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -962,15 +1019,15 @@
       <c r="E12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="19" t="s">
-        <v>54</v>
+      <c r="G12" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="20" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -983,15 +1040,15 @@
       <c r="E13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="19" t="s">
-        <v>55</v>
+      <c r="G13" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1004,15 +1061,15 @@
       <c r="E14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="19" t="s">
-        <v>56</v>
+      <c r="G14" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1021,11 +1078,11 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="19" t="s">
+      <c r="F15" s="12" t="s">
         <v>59</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1042,60 +1099,60 @@
       <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="19" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="13"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="13"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="13"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="13"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="10"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="10"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="10"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="10"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="10"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="10"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="10"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="10"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="11"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="10"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="10"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="10"/>
+      <c r="F32" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1120,4 +1177,17 @@
     <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904227A9-8220-4ECA-B365-60ECEE5A76EE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update UserForm: Replace alert with toast notifications . Implement address type management improvements, including handling for removed addresses and default type assignment.
</commit_message>
<xml_diff>
--- a/API_Mappings.xlsx
+++ b/API_Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learnings\fsm-webtools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F73709-5F3C-4BC7-9A34-B9564018FF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F11F889-EB88-4E1E-993B-624124898068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update UserForm: Enhance address type management with improved toast notifications for DEFAULT address handling. Update README with new endpoint information and modify API_Mappings.xlsx.
</commit_message>
<xml_diff>
--- a/API_Mappings.xlsx
+++ b/API_Mappings.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learnings\fsm-webtools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F11F889-EB88-4E1E-993B-624124898068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A125D8-9D3A-4871-B1A4-559EBBC0CE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GET" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="POST" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="110">
   <si>
     <t>Drop Down</t>
   </si>
@@ -289,12 +290,159 @@
   <si>
     <t>https://lely-fsm-dev.ifs.cloud/odata/currency?$select=currency,description,format_override&amp;$filter=active eq 'Y'</t>
   </si>
+  <si>
+    <t>Form Field</t>
+  </si>
+  <si>
+    <t>Json</t>
+  </si>
+  <si>
+    <t>FSM Table</t>
+  </si>
+  <si>
+    <t>FSM Column</t>
+  </si>
+  <si>
+    <t>Mapping</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>IFS User ID</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>SSO</t>
+  </si>
+  <si>
+    <t>Technician ID(MX)</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Lely Center(Access Group)</t>
+  </si>
+  <si>
+    <t>Allocated Team</t>
+  </si>
+  <si>
+    <t>FSM License</t>
+  </si>
+  <si>
+    <t>Mobile User</t>
+  </si>
+  <si>
+    <t>Dispatchable</t>
+  </si>
+  <si>
+    <t>Scheduling Resource</t>
+  </si>
+  <si>
+    <t>PSO System User</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>1-M</t>
+  </si>
+  <si>
+    <t>PERSON</t>
+  </si>
+  <si>
+    <t>FIRST_NAME</t>
+  </si>
+  <si>
+    <t>LAST_NAME</t>
+  </si>
+  <si>
+    <t>JOB_TITLE</t>
+  </si>
+  <si>
+    <t>ALLOCATED_TEAM</t>
+  </si>
+  <si>
+    <t>FSM_LICENSE</t>
+  </si>
+  <si>
+    <t>MOBILE_USER</t>
+  </si>
+  <si>
+    <t>SCHEDULING_RESOURCE</t>
+  </si>
+  <si>
+    <t>PERSON_ID</t>
+  </si>
+  <si>
+    <t>PERSON_Group)</t>
+  </si>
+  <si>
+    <t>PERSON_Group</t>
+  </si>
+  <si>
+    <t>PERSON_User</t>
+  </si>
+  <si>
+    <t>MOBILE_PHONE</t>
+  </si>
+  <si>
+    <t>MOBILE_TYPE</t>
+  </si>
+  <si>
+    <t>MOBILE_EMPLOYEE</t>
+  </si>
+  <si>
+    <t>MOBILE_LANGUAGE</t>
+  </si>
+  <si>
+    <t>MOBILE_CURRENCY</t>
+  </si>
+  <si>
+    <t>MOBILE_PLACES</t>
+  </si>
+  <si>
+    <t>MOBILE_ADDRESS</t>
+  </si>
+  <si>
+    <t>MOBILE_DISPATCHABLE</t>
+  </si>
+  <si>
+    <t>MOBILE_ROLES</t>
+  </si>
+  <si>
+    <t>sso_enabled</t>
+  </si>
+  <si>
+    <t>email_address/sso_user_id</t>
+  </si>
+  <si>
+    <t>external_reference</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,8 +481,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,8 +514,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -388,12 +555,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -424,6 +608,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -439,10 +625,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="3" builtinId="47"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -785,9 +985,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -826,7 +1029,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -838,15 +1041,15 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -858,11 +1061,11 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -875,15 +1078,15 @@
         <v>8</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -896,11 +1099,11 @@
         <v>8</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="18"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -913,11 +1116,11 @@
         <v>8</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="18"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -930,11 +1133,11 @@
         <v>8</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="18"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -947,11 +1150,11 @@
         <v>8</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="18"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -966,11 +1169,11 @@
       <c r="E9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="18"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -985,11 +1188,11 @@
       <c r="E10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="18"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1006,7 +1209,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1027,7 +1230,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1048,7 +1251,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1069,7 +1272,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1190,4 +1393,691 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6C4128-A0D9-4568-B324-F642B000A9F2}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="D1:J54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D1" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" s="21"/>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="21"/>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="J6" s="21"/>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="21"/>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="21"/>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="21"/>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="21"/>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" s="21"/>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" s="21"/>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="J27" s="21"/>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+    </row>
+    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+    </row>
+    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+    </row>
+    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+    </row>
+    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+    </row>
+    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+    </row>
+    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+    </row>
+    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+    </row>
+    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+    </row>
+    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove unused mutation and query functions.
</commit_message>
<xml_diff>
--- a/API_Mappings.xlsx
+++ b/API_Mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learnings\fsm-webtools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A125D8-9D3A-4871-B1A4-559EBBC0CE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B83B363-93D1-4E99-AA87-B0870642A245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="1920" windowWidth="28800" windowHeight="15345" tabRatio="340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GET" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Active = Y</t>
-  </si>
-  <si>
-    <t>Person Type</t>
   </si>
   <si>
     <t>Language</t>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>external_reference</t>
+  </si>
+  <si>
+    <t>License</t>
   </si>
 </sst>
 </file>
@@ -610,6 +610,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -625,19 +636,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -990,8 +990,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,13 +1019,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1041,16 +1041,16 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>51</v>
+      <c r="F2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -1061,252 +1061,252 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="18"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>52</v>
+      <c r="F4" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="20"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="20"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="F14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
@@ -1402,7 +1402,7 @@
   </sheetPr>
   <dimension ref="D1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1412,667 +1412,667 @@
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24" t="s">
+      <c r="I1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="22" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="16" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D2" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="25" t="s">
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="25" t="s">
+      <c r="H19" s="16"/>
+      <c r="I19" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D20" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="J3" s="21"/>
-    </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="25" t="s">
+      <c r="H20" s="16"/>
+      <c r="I20" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="J4" s="21"/>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D5" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="25" t="s">
+      <c r="H21" s="16"/>
+      <c r="I21" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D6" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="J6" s="21"/>
-    </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="J7" s="21"/>
-    </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="J8" s="21"/>
-    </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D9" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D10" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="21"/>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="21"/>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D12" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D13" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="J13" s="21"/>
-    </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D14" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="J14" s="21"/>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D15" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="J15" s="21"/>
-    </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="J16" s="21"/>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D17" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="J17" s="21"/>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D18" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="J18" s="21"/>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D19" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" s="21"/>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="J20" s="21"/>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="J21" s="21"/>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="J23" s="21"/>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21" t="s">
+      <c r="H27" s="16"/>
+      <c r="I27" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="J24" s="21"/>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D25" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="J25" s="21"/>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D26" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="J26" s="21"/>
-    </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D27" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="J27" s="21"/>
+      <c r="J27" s="16"/>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
     </row>
     <row r="34" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
     </row>
     <row r="38" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
     </row>
     <row r="44" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
     </row>
     <row r="45" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
     </row>
     <row r="46" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
     </row>
     <row r="47" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
     </row>
     <row r="48" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
     </row>
     <row r="49" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
     </row>
     <row r="50" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
     </row>
     <row r="51" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
     </row>
     <row r="52" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
     </row>
     <row r="53" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
     </row>
     <row r="54" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>